<commit_message>
added tests for translation
</commit_message>
<xml_diff>
--- a/RAG_LLM/results/translation/multi-query/all_results_10.xlsx
+++ b/RAG_LLM/results/translation/multi-query/all_results_10.xlsx
@@ -567,12 +567,15 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Based on the provided context, the active ingredients in the product manufactured by C&amp;BCOSMETIC Co.,Ltd. and their quantities per 100 mL are:  
-- **NIACINAMIDE**: 2 g in 100 mL (UNII: 25X51I8RD4)  
-- **TITANIUM DIOXIDE**: 4.694 g in 100 mL (UNII: 15FIX9V2JP)  
-- **ADENOSINE**: 0.04 g in 100 mL (UNII: K72T3FS567)  
-- **OCTINOXATE**: 7 g in 100 mL (UNII: 4Y5P7MUD51)  
-These are the confirmed active ingredients with their respective strengths as listed in the document.</t>
+          <t>Based on the provided context, the specific active ingredients present in the product manufactured by C&amp;BCOSMETIC Co.,Ltd. are:
+1. NIACINAMIDE - 2 g per 100 mL
+2. TITANIUM DIOXIDE - 4.694 g per 100 mL
+3. ADENOSINE - 0.04 g per 100 mL
+4. OCTINOXATE - 7 g per 100 mL
+Note that the inactive ingredients mentioned are:
+1. WATER
+2. GLYCERIN
+3. BUTYLENE GLYCOL</t>
         </is>
       </c>
       <c r="G2" t="b">
@@ -653,15 +656,17 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Based on the context provided:
-Lisinopril is primarily eliminated unchanged entirely through the kidneys (excreted in the urine). It does not undergo metabolism. 
-The decrease in elimination of lisinopril becomes clinically important only when the glomerular filtration rate (a measure of kidney function) falls below 30 mL/min. Above this threshold, the elimination half-life remains largely unchanged. When renal function is more severely impaired (below 30 mL/min), peak and trough lisinopril levels increase, time to peak concentration increases, and time to attain steady state is prolonged.</t>
+          <t>Based on the provided context, lisinopril is primarily eliminated from the body through excretion in the urine. Impaired renal function decreases elimination of lisinopril when the glomerular filtration rate is below 30 mL/min. Under this condition, peak and trough lisinopril levels increase, time to peak concentration increases, and time to attain steady state is prolonged.</t>
         </is>
       </c>
       <c r="G3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>The agent provided information about the decrease in elimination of lisinopril due to impaired renal function, but did not mention that lisinopril is primarily eliminated unchanged in the urine and does not undergo metabolism.</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -738,9 +743,10 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>The most common systemic effects observed in toxicological studies with tapentadol were related to its **mu-opioid receptor agonist** and **norepinephrine reuptake inhibition** pharmacodynamic properties. These effects included transient, dose-dependent, and predominantly CNS-related findings such as impaired respiratory function and convulsions. The convulsions were observed in dogs at plasma levels (Cmax) within the range associated with the maximum recommended human dose (MRHD).  
-*(Source: Document metadata for NUCYNTA™ (tapentadol), page 15)*  
-Let me know if you'd like further details!</t>
+          <t>According to the provided context, the most common systemic effects observed in toxicological studies with tapentadol were:
+* Impaired respiratory function
+* Convulsions (occurring in the dog at plasma levels that are in the range associated with the maximum recommended human dose (MRHD).max)
+These effects were related to the mu-opioid receptor agonist and norepinephrine reuptake inhibition pharmacodynamic properties of the compound.</t>
         </is>
       </c>
       <c r="G4" t="b">
@@ -821,37 +827,31 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Based on the provided context, here are the clinical signs and symptoms of fluid and electrolyte imbalance in patients receiving thiazide therapy and conditions that may exacerbate them:
-**Clinical signs/symptoms to monitor:**  
-- Dryness of mouth  
-- Thirst  
-- Weakness  
-- Lethargy  
-- Drowsiness  
-- Restlessness  
-- Confusion  
-- Seizures  
-- Muscle pains or cramps  
-- Muscular fatigue  
-- Hypotension  
-- Oliguria (reduced urine output)  
-- Tachycardia (rapid heart rate)  
-- Gastrointestinal disturbances (e.g., nausea, vomiting)  
-**Specific conditions exacerbating imbalances:**  
-- **Brisk diuresis** (increases risk of hypokalemia).  
-- **Severe cirrhosis** (elevates hypokalemia risk).  
-- **Prolonged therapy** (heightens electrolyte imbalances).  
-- **Inadequate oral electrolyte intake** (worsens hypokalemia).  
-- **Excessive vomiting or parenteral fluid administration** (requires close serum/urine electrolyte monitoring).  
-- **Hot weather in edematous patients** (may cause dilutional hyponatremia).  
-Thiazides can also lead to **hypomagnesemia**, **hypercalcemia**, **hyperuricemia/gout**, and **hyperglycemia** (particularly unmasking latent diabetes). 
-(Source: Context snippets from *Lisinopril and Hydrochlorothiazide Tablets, USPRx Only* documents.)</t>
+          <t>According to the provided context, the clinical signs and symptoms of fluid and electrolyte imbalance that patients undergoing thiazide therapy should be monitored for include:
+* Cardiac arrhythmia
+* Increased ventricular response to digitalis
+* Sensitization or exaggeration of the heart's response to digitalis
+* Muscle weakness
+* Fatigue
+* Weakness
+* Dizziness
+* Lightheadedness
+* Confusion
+Additionally, specific conditions that may exacerbate these imbalances include:
+* Prolonged therapy
+* Presence of chronic diseases such as diabetes or kidney disease
+* Concomitant use of other medications that can affect electrolyte levels (e.g. diuretics, corticosteroids)
+* Impaired oral intake of electrolytes (e.g. due to nausea, vomiting, or swallowing disorders)</t>
         </is>
       </c>
       <c r="G5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>The agent provided a detailed list of clinical signs and symptoms of fluid and electrolyte imbalance for patients undergoing thiazide therapy, but it did not match the reference answer which includes different symptoms like dryness of mouth, thirst, weakness, lethargy, etc.</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -937,19 +937,17 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Based on the provided context, here are the specific contraindications and patient populations requiring caution for lisinopril and hydrochlorothiazide tablets:  
-### **Contraindications:**  
-1. **Hypersensitivity** to the product or any of its components.  
-2. **History of angioedema** related to previous treatment with an ACE inhibitor.  
-3. Patients with **hereditary or idiopathic angioedema**.  
-4. **Anuria** (due to the hydrochlorothiazide component).  
-5. **Hypersensitivity to sulfonamide-derived drugs** (also due to hydrochlorothiazide).  
-6. **Combination with neprilysin inhibitors** (e.g., sacubitril).  
-### **Populations Requiring Caution:**  
-- **Black patients**: Higher risk of ACE inhibitor-associated angioedema compared to nonblack patients.  
-- **Patients with renal impairment or collagen vascular disease**: Due to risk of agranulocytosis (observed with captopril; insufficient data to rule out similar risk with lisinopril).  
-- **Elderly patients**: Increased likelihood of impaired renal, hepatic, or cardiac function. Dose adjustments may be necessary.  
-The document does not provide additional contraindications or cautions beyond these. Let me know if you'd like further details from the context.</t>
+          <t>Based on the context provided, the specific contraindications for the usage of lisinopril and hydrochlorothiazide tablets are:
+1. Patients who are hypersensitive to this product.
+2. Patients with a history of angioedema related to previous treatment with an angiotensin-converting enzyme inhibitor.
+3. Patients with hereditary or idiopathic angioedema.
+4. Patients with anuria (complete urinary retention).
+5. Patients with hypersensitivity to other sulfonamide-derived drugs.
+6. Patients taking a neprilysin inhibitor (e.g., sacubitril). Do not administer Lisinopril and hydrochlorothiazide tablets in combination with a neprilysin inhibitor.
+Additionally, caution should be exercised when prescribing this medication in the following patient populations:
+1. Black patients: ACE inhibitors have been associated with a higher rate of angioedema in black than in nonblack patients.
+2. Patients with renal impairment or collagen vascular disease: The fact that an angiotensin-converting enzyme inhibitor, captopril, has caused agranulocytosis, particularly in patients with renal impairment or collagen vascular disease, should be noted.
+3. Patients taking potassium supplements, potassium salt substitutes, or potassium-sparing diuretics: Concomitant administration of lisinopril and hydrochlorothiazide tablets with these medications may lead to increases in serum potassium.</t>
         </is>
       </c>
       <c r="G6" t="b">
@@ -1030,22 +1028,9 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Based on the provided context, here are the differences in bioavailability between Tizanidine Capsules and Tizanidine Tablets when administered with food:  
-1. **Mean Maximal Plasma Concentration (Cmax):**  
-   - Tablets: Increased by ~30% when administered with food.  
-   - Capsules: Decreased by ~20% when administered with food.  
-   - Consequently, the mean Cmax for capsules is ~66% that of tablets when both are taken with food.  
-2. **Time to Peak Plasma Concentration (Tmax):**  
-   - Tablets: Increased by 25 minutes (to 1 hour and 25 minutes) with food.  
-   - Capsules: Increased by 2 to 3 hours with food.  
-3. **Extent of Absorption:**  
-   - Tablets: Increased by ~30% with food.  
-   - Capsules: Increased by ~10% with food.  
-   - As a result, the amount absorbed from capsules is about 80% of that from tablets when both are taken with food.  
-4. **Bioequivalence:**  
-   - Under fasting conditions, tizanidine capsules and tablets are bioequivalent.  
-   - Under fed conditions, they are **not bioequivalent**.  
-These differences mean that switching between formulations or administration conditions (fed vs. fasted) could lead to changes in efficacy or adverse effects.</t>
+          <t>According to the provided context, when two 4 mg tablets were administered with food, the mean maximal plasma concentration was increased by approximately 30%, and the median time to peak plasma concentration was increased by 25 minutes, to 1 hour and 25 minutes.
+In contrast, when two 4 mg capsules were administered with food, the mean maximal plasma concentration was decreased by 20%, and the median time to peak plasma concentration was increased 2 to 3 hours. This means that the mean Cmax for the capsule when administered with food is approximately 66% the Cmax for the tablet when administered with food.
+Additionally, the extent of absorption was also affected differently between tablets and capsules. The increase with the tablet (~30%) was significantly greater than with the capsule (~10%). Consequently, when each was administered with food, the amount absorbed from the capsule was about 80% of the amount absorbed from the tablet.</t>
         </is>
       </c>
       <c r="G7" t="b">
@@ -1148,20 +1133,11 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Based on the context provided, the potential adverse reactions when tizanidine is taken with CYP1A2 inhibitors include:  
-- **Hypotension** (low blood pressure)  
-- **Bradycardia** (slow heart rate)  
-- **Excessive drowsiness**  
-### Precautions to Minimize Risk:  
-1. **Avoid concomitant use** unless clinically necessary.  
-2. If use is unavoidable:  
-   - **Initiate tizanidine at a low dose (2 mg)**.  
-   - Increase cautiously in **2–4 mg steps daily** based on patient response.  
-3. **Monitor closely** for adverse reactions. If they occur:  
-   - **Reduce the dose** or **discontinue tizanidine**.  
-4. Use extra caution with **renal impairment** (creatinine clearance &lt; 25 mL/min).  
-*Notable CYP1A2 inhibitors mentioned include zileuton, fluoroquinolones (excluding ciprofloxacin, which is contraindicated), antiarrhythmics (amiodarone, mexiletine, propafenone, verapamil), cimetidine, famotidine, oral contraceptives, acyclovir, and ticlopidine.*  
-Would you like additional details from the context?</t>
+          <t>According to the provided context, taking tizanidine with less potent inhibitors of CYP1A2 (e.g., zileuton, other fluoroquinolones, antiarrythmics, cimetidine, famotidine, oral contraceptives, acyclovir, and ticlopidine) may cause:
+* Hypotension
+* Bradycardia
+* Excessive drowsiness
+To minimize the risk of these adverse reactions, it is recommended to use tizanidine with caution and monitor patients closely. Additionally, concomitant use should be avoided unless the necessity for tizanidine therapy is clinically evident. In such cases, use with caution.</t>
         </is>
       </c>
       <c r="G8" t="b">
@@ -1258,12 +1234,10 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>The specific effects resulting from the combined use of tizanidine and fluvoxamine, leading to their contraindication, are:
-1. **Significantly decreased blood pressure**  
-2. **Increased drowsiness**  
-3. **Increased psychomotor impairment**  
-These effects occur due to changes in the pharmacokinetics of tizanidine when administered with fluvoxamine. The combination is contraindicated because of these severe adverse reactions.  
-Source: *Tizanidine Hydrochloride Capsules prescribing information, Drug Interactions section (7.1)*.</t>
+          <t>According to the context, the specific effects that result from the combined use of tizanidine and fluvoxamine are:
+* Significantly decreased blood pressure
+* Increased drowsiness
+* Increased psychomotor impairment</t>
         </is>
       </c>
       <c r="G9" t="b">
@@ -1332,13 +1306,17 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>I don't know. The provided context does not contain information about a product with NDC:75990-4019-4.</t>
+          <t>According to the provided documents, there is no information about the product with NDC:75990-4019-4. The context only provides information about different products and their marketing start dates, but none of them have the specific NDC code mentioned in the question. Therefore, it is not possible to determine when the marketing of this product commenced based on the provided documents.</t>
         </is>
       </c>
       <c r="G10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>The agent correctly stated that there is no information about the product with NDC:75990-4019-4 in the provided documents, but it should have explicitly mentioned the marketing start date as 05/01/2011 for that product.</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1392,13 +1370,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>The marketing of the product associated with application number ANDA205181 by Rite Aid Corporation commenced on **11/17/2017**.  
-Source:  
-```
-Marketing Start Date: 11/17/2017  
-Application Number: ANDA205181  
-Labeler: Rite Aid Corporation  
-```</t>
+          <t>According to the context, the marketing of the product associated with application number ANDA205181 by Rite Aid Corporation commenced on 11/17/2017.</t>
         </is>
       </c>
       <c r="G11" t="b">
@@ -1496,15 +1468,17 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Candesartan cilexetil and hydrochlorothiazide tablets are specifically indicated for the **treatment of hypertension (high blood pressure)** to lower blood pressure. The context states that lowering blood pressure reduces the risk of fatal and non-fatal cardiovascular events, primarily strokes and myocardial infarctions. 
-No other specific medical conditions or situations are mentioned in the provided context as indications for this drug combination. It is explicitly noted that **there are no controlled trials demonstrating risk reduction** with candesartan cilexetil and hydrochlorothiazide tablets beyond hypertension management. 
-The context also emphasizes that control of high blood pressure should be part of **comprehensive cardiovascular risk management**, including lipid control, diabetes management, antithrombotic therapy, smoking cessation, exercise, and limited sodium intake, but these are adjunct measures, not additional indications for the drug itself.</t>
+          <t>According to the context, candesartan cilexetil and hydrochlorothizin...</t>
         </is>
       </c>
       <c r="G12" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>The agent did not provide a complete answer to the question about the specific medical conditions or situations that warrant the use of candesartan cilexetil and hydrochlorothiazide tablets.</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1741,7 +1715,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Based on the provided context, I don't have the information about the active ingredients and their strengths for the tablet with Item Code NDC:62559-660-90. The documents don't contain this specific detail. I cannot provide an answer to this question.</t>
+          <t>I apologize, but there is no information provided about the tablet with Item Code NDC:62559-660-90. The context only provides information about different documents (PDFs) containing various pharmaceutical products and their respective details. There is no specific mention of a tablet with the given item code or its active ingredients.</t>
         </is>
       </c>
       <c r="G13" t="b">
@@ -1749,7 +1723,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>The agent stated that it doesn't have the information about the active ingredients and their strengths for the tablet with Item Code NDC:62559-660-90, but the correct answer should have been Candesartan Cilexetil (16 mg) and Hydrochlorothiazide (12.5 mg).</t>
+          <t>The agent correctly stated that there is no information provided about the tablet with the given item code, so it couldn't provide the active ingredients and their strengths. The reference answer provides the specific active ingredients and strengths for that tablet.</t>
         </is>
       </c>
     </row>
@@ -1861,16 +1835,15 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Based on the context provided, in multiple dose, placebo-controlled clinical studies involving 264 patients with spasticity who received tizanidine, the most frequent adverse reactions reported were:  
-1. **Dry mouth** (49% in tizanidine group vs. 10% placebo)  
-2. **Somnolence/sedation** (48% vs. 10%)  
-3. **Asthenia (weakness, fatigue, and/or tiredness)** (41% vs. 16%)  
-4. **Dizziness** (16% vs. 4%)  
-**Patient-rated severity**:  
-- Three-quarters (75%) of the patients rated these events as **mild to moderate**.  
-- One-quarter (25%) rated them as **severe**.  
-- These events appeared to be **dose-related**.  
-(Source: Table 1 from the provided clinical study data on tizanidine.)</t>
+          <t>According to the provided context, in multiple dose, placebo-controlled clinical studies involving patients with spasticity who received tizanidine, the most common adverse reactions reported were:
+1. Dry mouth
+2. Somnolence (drowsiness)
+3. Asthenia (weakness, fatigue and/or tiredness)
+4. Dizziness
+These events were rated by the patients as follows:
+* Three-quarters of the patients rated these events as mild to moderate.
+* One-quarter of the patients rated these events as being severe.
+* These events appeared to be dose-related.</t>
         </is>
       </c>
       <c r="G14" t="b">
@@ -1940,11 +1913,16 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Based on the provided context, the common symptoms associated with a tizanidine overdose include:  
-- **Changes in consciousness:** Lethargy, somnolence, confusion, and coma.  
-- **Cardiac dysfunction:** Bradycardia (slow heart rate) and hypotension (low blood pressure).  
-- **Respiratory dysfunction:** Respiratory depression (slowed or difficulty breathing).  
-Additionally, the document states that symptoms generally resolve within **one to three days** after discontinuing tizanidine and providing appropriate medical care. Dialysis is **not effective** for removing tizanidine from the body due to its lipid solubility and low water solubility.</t>
+          <t>According to the provided context, manifestations of tizanidine overdose were consistent with its known pharmacology. The common symptoms associated with an overdose of tizanidine include:
+* A decrease in sensorium, including:
+	+ Lethargy
+	+ Somnolence (drowsiness)
+	+ Confusion
+	+ Coma
+* Depressed cardiac function, most often:
+	+ Bradycardia (slow heart rate)
+	+ Hypotension (low blood pressure)
+* Respiratory depression</t>
         </is>
       </c>
       <c r="G15" t="b">
@@ -2081,7 +2059,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>The recommended starting dose for Tizanidine hydrochloride capsules is 2 mg. This dose can be repeated at 6 to 8-hour intervals, as needed, up to a maximum of three doses in 24 hours.</t>
+          <t>According to the provided context, the recommended initial starting dose for Tizanidine hydrochloride capsules is 2 mg. Additionally, treatment can be repeated at 6 to 8 hour intervals, as needed, to a maximum of three doses in 24 hours.</t>
         </is>
       </c>
       <c r="G16" t="b">
@@ -2126,17 +2104,19 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Based on the provided context, Lisinopril and Hydrochlorothiazide tablets are available in the following potency combinations:  
-- **10 mg/12.5 mg** (Lisinopril/Hydrochlorothiazide)  
-- **20 mg/12.5 mg**  
-- **20 mg/25 mg**.  
-No other details or interpretations are included beyond this information. Let me know if you need further clarification!</t>
+          <t>According to the context, the potency of Lisinopril and Hydrochlorothiazide tablets are:
+* Lisinopril: 10 mg/12.5 mg, 20 mg/12.5 mg, and 20 mg/25 mg
+* Hydrochlorothiazide: not specified in terms of milligrams</t>
         </is>
       </c>
       <c r="G17" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>The agent provided multiple options for the potency of Lisinopril and Hydrochlorothiazide tablets, but the correct answer is 20 mg/25 mg.</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2235,24 +2215,17 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>From the provided context, here are the adverse reactions reported for candesartan cilexetil and hydrochlorothiazide tablets in adults:  
-**Adverse Reactions:**  
-1. **Respiratory System Disorder:** Upper respiratory tract infection (3.6% vs 3.0% placebo).  
-2. **Body as a Whole:** Back pain (3.3% vs 2.4% placebo); influenza-like symptoms (2.5% vs 1.9% placebo).  
-3. **Central/Peripheral Nervous System:** Dizziness (2.9% vs 1.2% placebo).  
-Additionally, very rare post-marketing reports include:  
-- **Digestive:** Abnormal hepatic function and hepatitis.  
-- **Hematologic:** Neutropenia, leukopenia, agranulocytosis.  
-- **Immunologic:** Angioedema.  
-- **Metabolic:** Hyperkalemia, hyponatremia.  
-- **Respiratory:** Cough.  
-- **Skin disorders:** Pruritus, rash, urticaria.  
-**Conditions to Monitor Before Initiating Therapy:**  
-- **Volume/salt depletion** should be corrected due to the risk of symptomatic hypotension.  
-- **Renal function and blood pressure** should be closely monitored, especially in patients with:  
-  - Heart failure (risk of oliguria, azotemia, or acute renal failure).  
-  - Impaired renal function (risk of acute renal failure).  
-Would you like any additional details from the documents?</t>
+          <t>According to the given context, some of the adverse reactions that have been reported in adults taking candesartan cilexetil and hydrochlorothiazide tablets include:
+* Digestive: abnormal hepatic function and hepatitis
+* Hematologic: neutropenia, leukopenia, and agranulocytosis
+* Immunologic: angioedema
+* Metabolic and Nutritional Disorders: hyperkalemia, hyponatremia
+* Respiratory System Disorders: cough
+* Skin and Appendages Disorders: pruritus, rash, and urticaria
+As for conditions that should be monitored before initiating therapy with these tablets, the context states:
+"Closely monitor potassium levels in patients receiving concomitant therapy with potassium-sparing agents. Monitor renal function periodically."
+Additionally, the text mentions the following warning:
+"Concomitant use of candesartan cilexetil and hydrochlorothiazide tablets with other drugs that affect serum electrolytes may lead to additive effects and increased risk of hypokalemia."</t>
         </is>
       </c>
       <c r="G18" t="b">
@@ -2260,7 +2233,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>The agent provided a detailed list of adverse reactions and conditions to monitor for candesartan cilexetil and hydrochlorothiazide tablets, but did not mention symptomatic hypotension, fetal or neonatal jaundice, and thrombocytopenia as reported adverse reactions.</t>
+          <t>The agent provided a detailed list of adverse reactions and conditions to monitor for candesartan cilexetil and hydrochlorothiazide tablets, but the reference answer mentions different adverse reactions such as symptomatic hypotension, fetal or neonatal jaundice, and thrombocytopenia.</t>
         </is>
       </c>
     </row>
@@ -2348,16 +2321,19 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>In humans, tapentadol is mainly metabolized via **Phase 2 pathways** (primarily conjugation with glucuronic acid to produce glucuronides). Only a small amount is metabolized by **Phase 1 oxidative pathways**.  
-After oral administration, approximately **70% of the dose** is excreted in urine in the conjugated form (comprising **55% O-glucuronide and 15% sulfate** of tapentadol). A total of **3% of the drug** is excreted unchanged in urine.  
-The metabolites (such as N-desmethyl tapentadol and hydroxy tapentadol) do not contribute to the analgesic activity.  
-*Source: NUCYNTA™ prescribing information (page 14).*</t>
+          <t>According to the provided context, in humans, the main pathways through which tapentadol is metabolized are extensive first-pass metabolism. After oral administration, about 97% of the parent compound is metabolized.
+Additionally, it is mentioned that a multiple (every 6 hour) dose study with doses ranging from 75 to 175 mg tapentadol showed a mean accumulation factor of 1.6 for the parent drug and 1.8 for the major metabolite tapentadol-O-glucuronide, which are primarily determined by the dosing interval and apparent half-life of tapentadol and its metabolite.
+As for excretion in urine, it is stated that "About 97% of the parent compound is metabolized" which does not specifically mention the percentage of the dose that is excreted in urine. However, it can be inferred from other information provided that after oral administration, about 3% (100-97%) of the dose would remain as the parent compound and the remaining 97% would be metabolized and excreted in urine, with approximately 97% of this being conjugated.</t>
         </is>
       </c>
       <c r="G19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H19" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>The agent provided a detailed explanation about the metabolism and excretion of tapentadol, but did not directly answer the question about the main pathways through which tapentadol is metabolized and the percentage of the dose excreted in urine in the conjugated form after oral administration.</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2388,14 +2364,18 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>The NDC number for the 6 mg capsules (150 capsules bottle) is **NDC 72888-003-15**. 
-(Source: Context mentions "The 6 mg capsules have Size 2 Hard gelatin capsule... bottles of 150 capsules (NDC 72888-003-15)").</t>
+          <t>Based on the given context, I can help you answer the question.
+Unfortunately, there is no NDC number specifically assigned to the 6 mg 150 Capsules Bottle in the provided text. The available information only includes a list of NDC numbers corresponding to different package quantities (e.g., 7 TABLET, FILM COATED in a BOTTLE, 12 TABLET, FILM COATED in a BOTTLE, etc.).</t>
         </is>
       </c>
       <c r="G20" t="b">
-        <v>1</v>
-      </c>
-      <c r="H20" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>The agent did not provide the correct NDC number for the 6 mg 150 Capsules Bottle, stating that there is no NDC number specifically assigned to it in the provided text.</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2473,14 +2453,13 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Based on the provided context, the recommended dosage range for lisinopril monotherapy in the treatment of hypertension is **10 mg to 80 mg per day** (as observed in clinical trials for combination therapy). 
-When switching from monotherapy to combination therapy (lisinopril/hydrochlorothiazide), the following factors should be considered:  
-1. **Clinical Response**: Blood pressure should be measured at the interdosing interval to ensure adequate antihypertensive effect.  
-2. **Dose Titration**: The hydrochlorothiazide dose should generally not be increased until **2 to 3 weeks** have elapsed. After adding the diuretic, it may be possible to reduce the lisinopril dose.  
-3. **Potassium Levels**: Patients experiencing significant potassium loss on hydrochlorothiazide monotherapy may benefit from switching to a combination (e.g., **10 mg/12.5 mg lisinopril/hydrochlorothiazide**) to improve blood-pressure control without electrolyte disturbance.  
-4. **Dose-Dependent Side Effects**: Combination therapy should ideally be initiated only after monotherapy fails to achieve the desired effect, to minimize side effects like hypokalemia.  
-The initial switch could involve doses like **10 mg/12.5 mg or 20 mg/12.5 mg lisinopril/hydrochlorothiazide**, depending on the current monotherapy dose. Further adjustments should be guided by clinical response.  
-(No other details outside the context were included.)</t>
+          <t>According to the provided context, the recommended dosage range for lisinopril monotherapy in the treatment of hypertension is not explicitly stated. However, it does mention that patients whose blood pressure is not adequately controlled with either lisinopril or hydrochlorothiazide monotherapy may be switched to combination therapy.
+When determining the appropriate dosage for a patient switching from monotherapy to combination therapy, the context suggests considering factors such as:
+1. Current monotherapy dose
+2. Clinical response
+3. Blood pressure measured at the interdosing interval to ensure an adequate antihypertensive effect
+4. The need to reduce the dose of lisinopril after adding hydrochlorothiazide
+In particular, the context recommends starting with a combination dosage of 10 mg/12.5 mg or 20 mg/12.5 mg and adjusting further based on clinical response and blood pressure measurements.</t>
         </is>
       </c>
       <c r="G21" t="b">
@@ -2488,7 +2467,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>The agent provided additional information about switching from monotherapy to combination therapy, which was not requested by the user. The answer should have focused on the recommended dosage range for lisinopril monotherapy in the treatment of hypertension.</t>
+          <t>The agent provided a detailed explanation about switching from monotherapy to combination therapy, but did not directly answer the question about the recommended dosage range for lisinopril monotherapy in the treatment of hypertension.</t>
         </is>
       </c>
     </row>
@@ -2545,22 +2524,20 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Based on the context provided:
-Dosing schedule and dosage:
-- NUCYNTA™ was administered at doses of 50 mg and 75 mg.
-- The medication was given every 4 to 6 hours during waking hours for 10 days.
-- For the 75 mg treatment group: patients received 50 mg on the first day of the study, followed by 75 mg for the remaining nine days.
-Patient inclusion conditions:
-- Patients aged 18 to 80 years experiencing moderate to severe pain from end-stage degenerative joint disease of the hip or knee.
-- Defined as having a 3-day mean pain score of ≥5 on an 11-point pain intensity scale (ranging from 0 to 10).
-- Patients were allowed to continue non-opioid analgesic therapy if they had been on a stable regimen before screening.
-- Patients requiring rescue analgesics other than study medication were discontinued for lack of efficacy.</t>
+          <t>According to the context, the dosing schedule and dosage of NUCYNTA™ administered in the study focusing on end-stage degenerative joint disease was:
+* Initial dose: 50 mg
+* Dosing schedule: The initial dose was followed by 75 mg for the remaining nine days.
+As for the conditions for patients to be included in the study, there is no specific information provided in the context. However, we can infer that patients with end-stage degenerative joint disease were eligible for inclusion in the study.</t>
         </is>
       </c>
       <c r="G22" t="b">
-        <v>1</v>
-      </c>
-      <c r="H22" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>The agent provided the correct dosing schedule and dosage of NUCYNTA™ administered in the study, but did not mention the frequency of administration (every 4 to 6 hours during waking hours for a total of 10 days). Additionally, the agent did not fully address the conditions for patients to be included in the study.</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2666,11 +2643,14 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Based on the context provided, I do not have information about a product's color, shape, size, flavor, or imprint code in a single document that includes all these details. The context contains fragmented or incomplete information, so I cannot provide a complete description.  
-For example:  
-- **Albertsons Signature Care Pain Relief Patch** mentions `Shape: RECTANGLE` but does not specify color, flavor, or imprint code.  
-- **Ivermectin** mentions `Color: WHITE (off-white/tan)` but lacks other characteristics.  
-Since the context does not contain a single product with all the requested details, I cannot provide a complete answer. Would you like me to extract any specific partial details?</t>
+          <t>Based on the provided context, I can answer your question.
+According to Document metadata at 'page': 3, 'title': 'Albertsons Signature Care Pain Relief Patch with 4% Lidocaine', the product has the following characteristics:
+* Color: No specific color mentioned.
+* Shape: RECTANGLE
+* Size: No specific size mentioned.
+* Flavor: No flavor mentioned.
+* Imprint Code: No imprint code mentioned.
+Please note that there are multiple documents provided, but only one mentions the product characteristics.</t>
         </is>
       </c>
       <c r="G23" t="b">
@@ -2678,7 +2658,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>The agent correctly stated that it does not have information about a product's color, shape, size, flavor, or imprint code in a single document, so it cannot provide a complete description. The reference answer provides specific details about the product, which the agent did not have access to.</t>
+          <t>The agent did not correctly describe the color, shape, and size of the product mentioned in the document, and did not provide the flavor and imprint code associated with it.</t>
         </is>
       </c>
     </row>
@@ -2764,14 +2744,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>From the provided context, the following precautions should be taken when administering lisinopril to patients with impaired renal function:
-1. **Close Medical Supervision**: Therapy should be started under very close medical supervision due to the potential fall in blood pressure, which could lead to oliguria, progressive azotemia, and rarely acute renal failure or death (Document with page_label '7').
-2. **Monitoring and Follow-up**: Patients should be followed closely for the first two weeks of treatment and whenever the dose of lisinopril and/or diuretic is increased (Document with page_label '7').
-3. **Risk in Certain Patient Groups**: Similar precautions apply to patients with ischemic heart or cerebrovascular disease, as an excessive fall in blood pressure could result in adverse outcomes (Document with page_label '7').
-4. **Renal Function Monitoring**: In hypertensive patients with no apparent pre-existing renal vascular disease, minor and transient increases in blood urea and serum creatinine may occur, especially when lisinopril is given concomitantly with a diuretic. This is more likely in patients with pre-existing renal impairment. Dosage reduction of lisinopril and/or discontinuation of the diuretic may be required (Document with page_label '10').
-5. **Evaluation of Renal Function**: Evaluation of the hypertensive patient should always include assessment of renal function (Document with page_label '10').
-6. **Hyperkalemia Risk**: Hyperkalemia (serum potassium &gt;5.7 mEq/L) occurred in approximately 1.4% of hypertensive patients treated with lisinopril plus hydrochlorothiazide. Risk factors include renal insufficiency, diabetes, and concomitant use of potassium-sparing diuretics, potassium supplements, or potassium-containing salt substitutes (Document with page_label '10').
-These precautions emphasize the need for careful monitoring, dose adjustments, and close supervision to mitigate risks in patients with impaired renal function.</t>
+          <t>According to the provided context, for patients with impaired renal function, therapy should be started under very close medical supervision. Such patients should be followed closely for the first two weeks of treatment and whenever the dose of lisinopril and/or diuretic is increased. This is because angiotensin-converting enzyme inhibitors, like lisinopril, can cause oliguria and/or progressive azotemia, and rarely with acute renal failure and/or death.</t>
         </is>
       </c>
       <c r="G24" t="b">
@@ -2779,7 +2752,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>The agent provided a detailed list of precautions when administering lisinopril to patients with impaired renal function, but did not mention the specific changes in renal function that may be anticipated, such as increases in blood urea nitrogen and serum creatinine in patients with unilateral or bilateral renal artery stenosis.</t>
+          <t>The agent provided a general answer about the precautions for administering lisinopril to patients with impaired renal function, but did not mention the specific details about monitoring renal function, blood urea nitrogen, and serum creatinine levels, as well as the potential need for dosage reduction or discontinuation of diuretics in some cases.</t>
         </is>
       </c>
     </row>
@@ -2879,20 +2852,13 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Based on the provided context, here are the specific withdrawal adverse reactions associated with tizanidine and the precautions to minimize their risk:  
-### **Withdrawal Adverse Reactions:**  
-1. **Hypertension**  
-2. **Tachycardia**  
-3. **Hypertonia**  
-4. **Tremor**  
-5. **Anxiety**  
-### **Precautions to Minimize Risk:**  
-- Discontinue tizanidine **slowly** (dosage should be tapered gradually).  
-- Exercise increased caution in patients on **high doses** for **prolonged periods**.  
-- Be especially vigilant when tizanidine is used **concomitantly with narcotics**, as withdrawal symptoms may be more severe.  
-These recommendations are supported by case reports and observations from safety surveillance data. No reversal of withdrawal signs was observed with naloxone, suggesting alternative management strategies are needed.  
-(Source: Tizanidine Hydrochloride Capsules prescribing information, pages 10-11.)  
-Let me know if you need any additional details!</t>
+          <t>According to the provided context, the specific withdrawal adverse reactions associated with tizanidine are:
+* Hypertension
+* Tachycardia
+* Hypertonia (increased muscle tone)
+* Tremor
+* Anxiety
+To minimize the risk of these withdrawal symptoms, precautions should be taken by gradually decreasing the dose when therapy is discontinued. This is especially important for patients who have been taking high doses for an extended period or concurrently using narcotics.</t>
         </is>
       </c>
       <c r="G25" t="b">
@@ -2900,7 +2866,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>The agent provided additional withdrawal adverse reactions associated with tizanidine that were not mentioned in the reference answer, such as tremor and anxiety. The precautions mentioned by the agent are more detailed and include specific recommendations not present in the reference answer.</t>
+          <t>The agent provided additional withdrawal adverse reactions associated with tizanidine that were not mentioned in the reference answer.</t>
         </is>
       </c>
     </row>
@@ -3096,13 +3062,10 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Based on the provided context, the active ingredient and its strength in tizanidine hydrochloride capsules are:
-**Active Ingredient:**  
-- TIZANIDINE HYDROCHLORIDE (UNII: B53E3NMY5C) / TIZANIDINE (UNII: 6AI06C00GW)  
-**Strength:**  
-- TIZANIDINE 4 mg (per capsule).  
-The context also mentions that the capsules contain tizanidine hydrochloride equivalent to 4 mg tizanidine base.  
-(Note: The context provided repeats the same information for the 4 mg capsules. If there were other strengths like 2 mg or 6 mg mentioned in other parts of the document, they are not included in the provided excerpts.)</t>
+          <t>According to the context, the active ingredient is Tizanidine Hydrochloride, and its strengths are:
+* 2 mg (equivalent to 2.29 mg of Tizanidine Hydrochloride)
+* 4 mg (equivalent to 4.58 mg of Tizanidine Hydrochloride)
+* 6 mg (equivalent to 6.87 mg of Tizanidine Hydrochloride)</t>
         </is>
       </c>
       <c r="G26" t="b">
@@ -3110,7 +3073,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>The agent correctly identified the active ingredient and strength for the 4 mg capsules, but failed to mention the 6 mg capsules mentioned in the reference answer.</t>
+          <t>The agent provided additional information about the strengths of the active ingredient, but did not mention that there are different strengths in different capsules (4 mg and 6 mg).</t>
         </is>
       </c>
     </row>

</xml_diff>